<commit_message>
further specify mandatory fields
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE063935-7B6A-4900-9F65-AAA054DFCB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3DE775-6A5E-4255-AC5D-039203997EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>version</t>
   </si>
   <si>
     <t>doi</t>
@@ -134,9 +128,6 @@
 </t>
   </si>
   <si>
-    <t>https://www.cognitiveatlas.org/concepts/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cognitive Atlas task(s)
 </t>
   </si>
@@ -154,19 +145,10 @@
 # BOLD field are mandatory</t>
   </si>
   <si>
-    <t>internet link</t>
-  </si>
-  <si>
     <t>https://bids-specification.readthedocs.io/en/stable/modality-agnostic-files.html#dataset_descriptionjson</t>
   </si>
   <si>
     <t>Number of biological males</t>
-  </si>
-  <si>
-    <t>BIDS Modalities</t>
-  </si>
-  <si>
-    <t>https://bids-specification.readthedocs.io/en/stable/glossary.html#modality-common_principles</t>
   </si>
   <si>
     <t>Phenotyping Tests</t>
@@ -187,6 +169,36 @@
   <si>
     <t>ORCID</t>
   </si>
+  <si>
+    <t>like the BIDS README.txt</t>
+  </si>
+  <si>
+    <t>internet link/desription</t>
+  </si>
+  <si>
+    <t>This is how it will show in the data catalogue</t>
+  </si>
+  <si>
+    <t>https://bids-specification.readthedocs.io/en/stable/common-principles.html</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>useful for searches</t>
+  </si>
+  <si>
+    <t>a set of keywords</t>
+  </si>
+  <si>
+    <t>BIDS Dataset type</t>
+  </si>
+  <si>
+    <t>BIDS data type</t>
+  </si>
+  <si>
+    <t>https://www.cognitiveatlas.org/concepts</t>
+  </si>
 </sst>
 </file>
 
@@ -195,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +225,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -220,35 +247,41 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -623,36 +656,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -661,96 +679,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -759,32 +756,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1001,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1015,111 +1048,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>37</v>
+      <c r="A1" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="18" t="s">
-        <v>15</v>
+      <c r="B3" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="19" t="s">
-        <v>16</v>
+      <c r="B4" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>17</v>
+      <c r="A5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="19" t="s">
-        <v>18</v>
+      <c r="A6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="19"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="C9" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="21"/>
+    <row r="10" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1139,13 +1163,11 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="21"/>
+      <c r="A11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="68"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1165,11 +1187,13 @@
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="21"/>
+      <c r="A12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1188,14 +1212,12 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="21"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="68"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1215,13 +1237,13 @@
       <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="21"/>
+      <c r="A14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1241,13 +1263,13 @@
       <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="38"/>
+      <c r="A15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1266,30 +1288,56 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="22"/>
+    <row r="16" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{C5081CDB-9A30-4468-997D-60A4E3CB7934}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{DC3D51A7-F430-4DCF-A05F-7444C65A5483}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{6C3C6167-70C0-4DAB-8771-CD685858FA99}"/>
-    <hyperlink ref="B13" r:id="rId4" xr:uid="{9E55DD76-FBD3-4495-9E56-F5D4F3842017}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{042E520D-DC3A-465C-A1A0-E0407B43AE55}"/>
-    <hyperlink ref="B5" r:id="rId6" location="dataset_descriptionjson" xr:uid="{F6C4DD7F-BDF1-415D-A415-DE85F43495B0}"/>
-    <hyperlink ref="B7" r:id="rId7" location="modality-common_principles" xr:uid="{FC9DB523-70D6-417A-B2D7-B4597C9DE102}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{C5081CDB-9A30-4468-997D-60A4E3CB7934}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{DC3D51A7-F430-4DCF-A05F-7444C65A5483}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{6C3C6167-70C0-4DAB-8771-CD685858FA99}"/>
+    <hyperlink ref="B14" r:id="rId4" xr:uid="{9E55DD76-FBD3-4495-9E56-F5D4F3842017}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{042E520D-DC3A-465C-A1A0-E0407B43AE55}"/>
+    <hyperlink ref="B6" r:id="rId6" location="dataset_descriptionjson" xr:uid="{F6C4DD7F-BDF1-415D-A415-DE85F43495B0}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{FC9DB523-70D6-417A-B2D7-B4597C9DE102}"/>
   </hyperlinks>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1310,49 +1358,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
-        <v>46</v>
+      <c r="A1" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
-        <v>41</v>
+      <c r="A3" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="41" t="s">
-        <v>24</v>
+      <c r="A7" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
-        <v>47</v>
+      <c r="A9" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1378,7 +1426,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1389,18 +1437,18 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="70"/>
+      <c r="A4" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="58"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2423,7 +2471,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -2434,49 +2482,49 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>49</v>
+      <c r="B3" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="15"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="15"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3496,7 +3544,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -3507,25 +3555,25 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="54" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4554,7 +4602,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -4565,30 +4613,30 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="63" t="s">
+      <c r="A3" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="51" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="61"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="45"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
xlsx template with ag range
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3DE775-6A5E-4255-AC5D-039203997EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86407B86-38FA-469B-9A7A-F073400CFE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_info" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -199,6 +199,12 @@
   <si>
     <t>https://www.cognitiveatlas.org/concepts</t>
   </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Age range [min max]</t>
+  </si>
 </sst>
 </file>
 
@@ -207,11 +213,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -656,17 +669,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -679,75 +692,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -756,67 +769,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1036,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1346,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BA1306-610D-41AB-9268-9BD73CE522CE}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,8 +1420,20 @@
       </c>
       <c r="B7" s="8"/>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
use a priori PN-ID and DOI
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222670D2-ED49-4DB0-9F48-709ECA8BEC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4FBC14-5546-4298-AD58-82FDF228B42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_info" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>e.g. anat, func, fmap</t>
+  </si>
+  <si>
+    <t>PublicNeuro intra (for our record)</t>
+  </si>
+  <si>
+    <t>PN ID</t>
+  </si>
+  <si>
+    <t>DOI</t>
   </si>
 </sst>
 </file>
@@ -213,11 +225,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -676,17 +695,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -699,74 +718,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -775,78 +788,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1064,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,86 +1120,88 @@
       <c r="C2" s="68"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="73" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="74" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="74" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="72"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="74" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="74" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1193,11 +1221,11 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="70"/>
-      <c r="C11" s="15"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1217,13 +1245,13 @@
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1243,11 +1271,11 @@
       <c r="T12" s="3"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="70"/>
-      <c r="C13" s="15"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1267,13 +1295,13 @@
       <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1293,13 +1321,13 @@
       <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1319,13 +1347,13 @@
       <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1345,11 +1373,30 @@
       <c r="T16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="77" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1388,7 +1435,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1399,7 +1446,7 @@
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="8"/>
@@ -1423,25 +1470,25 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="60" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="28" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1479,18 +1526,18 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="57"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2524,48 +2571,48 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="34"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3597,25 +3644,25 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="51" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4630,7 +4677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4655,30 +4702,30 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="32"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
doi with a .
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5973BD4-6BA0-4E35-9AF9-371236F2EF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67562E47-A283-49DF-8D95-F5FF46519C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,9 +219,6 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>https://doi.org/1070883/XXXX</t>
-  </si>
-  <si>
     <t>PN00000X</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>your future DOI</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.70883/XXXX</t>
   </si>
 </sst>
 </file>
@@ -874,6 +874,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -903,9 +906,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,20 +1137,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="76" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="72"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="76"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -1187,7 +1187,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="57"/>
       <c r="C6" s="64">
@@ -1198,7 +1198,7 @@
       <c r="A7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="80" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="64" t="s">
@@ -1209,7 +1209,7 @@
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="80"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="64" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="78" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="13"/>
@@ -1266,7 +1266,7 @@
       <c r="A12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="14"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1290,7 +1290,7 @@
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="78" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="14"/>
@@ -1316,7 +1316,7 @@
       <c r="A14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="14"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1432,22 +1432,22 @@
       <c r="A22" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="81" t="s">
-        <v>64</v>
+      <c r="B22" s="71" t="s">
+        <v>63</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="68" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" s="68" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3697,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
make one utility for all metadata listing
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E4D91E-4A6C-4ABD-99D9-F2650FD2BB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B436A338-60B8-4CC0-8A69-BDA3FDEB4AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>https://doi.org/10.70883/XXXX</t>
+  </si>
+  <si>
+    <t>1 by default</t>
   </si>
 </sst>
 </file>
@@ -244,11 +247,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -720,17 +730,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,68 +753,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -813,63 +823,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -877,35 +887,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1125,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,7 +1202,9 @@
       <c r="A6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="C6" s="64">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
excel file now includes DUA and export takes care of it
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B436A338-60B8-4CC0-8A69-BDA3FDEB4AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C7504D-2231-4D80-87F2-884C12260827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,11 @@
     <sheet name="dataset_info" sheetId="1" r:id="rId1"/>
     <sheet name="participants_info" sheetId="6" r:id="rId2"/>
     <sheet name="data-controller" sheetId="2" r:id="rId3"/>
-    <sheet name="authors" sheetId="3" r:id="rId4"/>
-    <sheet name="dataset curators" sheetId="7" r:id="rId5"/>
-    <sheet name="funding" sheetId="4" r:id="rId6"/>
-    <sheet name="publications" sheetId="5" r:id="rId7"/>
+    <sheet name="DUA" sheetId="8" r:id="rId4"/>
+    <sheet name="authors" sheetId="3" r:id="rId5"/>
+    <sheet name="dataset curators" sheetId="7" r:id="rId6"/>
+    <sheet name="funding" sheetId="4" r:id="rId7"/>
+    <sheet name="publications" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -238,6 +239,33 @@
   </si>
   <si>
     <t>1 by default</t>
+  </si>
+  <si>
+    <t>Restrictions</t>
+  </si>
+  <si>
+    <t>only users from EU and adequate countries + data controller oversight</t>
+  </si>
+  <si>
+    <t>i.e.</t>
+  </si>
+  <si>
+    <t>None (CCBY)</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>only users from EU and adequate countries</t>
+  </si>
+  <si>
+    <t>Institution of users from non EU or adequate countries must be able to sign standard contractual clauses</t>
+  </si>
+  <si>
+    <t>Institution of users from non EU or adequate countries must be able to sign standard contractual clauses  + data controller oversight</t>
+  </si>
+  <si>
+    <t>Please copy/paste here your DUA, it will be displayed as a tab on the website -- of course the text/doc/pdf file you use for DUA is the one user mst sign, this field is for display purpose of your terms</t>
   </si>
 </sst>
 </file>
@@ -247,11 +275,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -407,6 +449,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -730,17 +793,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -753,68 +816,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -823,63 +886,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -887,38 +948,58 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1139,7 +1220,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,29 +1231,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="85" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="73"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="77"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="61" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1180,10 +1261,10 @@
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="62" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1191,10 +1272,10 @@
       <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="62" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1202,10 +1283,10 @@
       <c r="A6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="62">
         <v>1</v>
       </c>
     </row>
@@ -1213,10 +1294,10 @@
       <c r="A7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="62" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1224,8 +1305,8 @@
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="64" t="s">
+      <c r="B8" s="90"/>
+      <c r="C8" s="62" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1236,7 +1317,7 @@
       <c r="B9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="62" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1255,7 +1336,7 @@
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="87" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="13"/>
@@ -1281,7 +1362,7 @@
       <c r="A12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="79"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="14"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1305,7 +1386,7 @@
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="87" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="14"/>
@@ -1331,7 +1412,7 @@
       <c r="A14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="79"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="14"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1434,20 +1515,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="19"/>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="63" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="67" t="s">
+      <c r="A21" s="65" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="69" t="s">
         <v>63</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1455,13 +1536,13 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="66" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1494,7 +1575,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1508,7 +1589,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="75" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8"/>
@@ -1544,16 +1625,16 @@
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="57"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
@@ -1570,7 +1651,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1594,18 +1675,18 @@
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="55"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2611,11 +2692,121 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B86173-1A43-48AD-9DDE-136087F17F2C}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="92.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="A1" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="B3" s="92"/>
+      <c r="D3" s="74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="92"/>
+      <c r="D4" s="72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="B5" s="92"/>
+      <c r="D5" s="74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="92"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="92"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="92"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="92"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="92"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="92"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="92"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="92"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="92"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="92"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="92"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="92"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="92"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B19"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select from drop down menu" sqref="B1" xr:uid="{25815616-16C1-4ABC-AD84-B7D71FCF238B}">
+      <formula1>$D$1:$D$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2651,7 +2842,7 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
+      <c r="A4" s="79"/>
       <c r="B4" s="33"/>
       <c r="C4" s="34"/>
       <c r="D4" s="1"/>
@@ -3683,12 +3874,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845FEB05-2599-4045-8FC7-E4172C92513F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3716,28 +3907,28 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
-      <c r="B4" s="69"/>
+      <c r="A4" s="79"/>
+      <c r="B4" s="80"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="32"/>
-      <c r="B5" s="69"/>
+      <c r="B5" s="67"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="35"/>
-      <c r="B6" s="69"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="32"/>
-      <c r="B7" s="69"/>
+      <c r="B7" s="67"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="32"/>
-      <c r="B8" s="69"/>
+      <c r="B8" s="67"/>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="36"/>
-      <c r="B9" s="70"/>
+      <c r="B9" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3745,12 +3936,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4803,7 +4994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
@@ -4835,7 +5026,7 @@
       <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="59" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="47" t="s">
@@ -4847,7 +5038,7 @@
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46"/>
-      <c r="B4" s="62"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="46"/>
       <c r="D4" s="30"/>
     </row>

</xml_diff>

<commit_message>
export all UCBJ Leuven (+ DUA fix)
</commit_message>
<xml_diff>
--- a/import/PublicnEUro_record.xlsx
+++ b/import/PublicnEUro_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C7504D-2231-4D80-87F2-884C12260827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983252D5-046F-436C-9246-BA86E491278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_info" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t># bold fields are required</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>Please copy/paste here your DUA, it will be displayed as a tab on the website -- of course the text/doc/pdf file you use for DUA is the one user mst sign, this field is for display purpose of your terms</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -2693,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B86173-1A43-48AD-9DDE-136087F17F2C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2706,48 +2712,53 @@
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.45">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="A2" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D2" s="78" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B3" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D3" s="72" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.45">
-      <c r="B3" s="92"/>
-      <c r="D3" s="74" t="s">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="B4" s="92"/>
+      <c r="D4" s="74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="92"/>
-      <c r="D4" s="72" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="92"/>
+      <c r="D5" s="72" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.45">
-      <c r="B5" s="92"/>
-      <c r="D5" s="74" t="s">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.45">
+      <c r="B6" s="92"/>
+      <c r="D6" s="74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="92"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="92"/>
@@ -2788,13 +2799,16 @@
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="92"/>
     </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="92"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:B19"/>
+    <mergeCell ref="B3:B20"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select from drop down menu" sqref="B1" xr:uid="{25815616-16C1-4ABC-AD84-B7D71FCF238B}">
-      <formula1>$D$1:$D$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select from drop down menu" sqref="B2" xr:uid="{25815616-16C1-4ABC-AD84-B7D71FCF238B}">
+      <formula1>$D$2:$D$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>